<commit_message>
ensure that we read the underlying data values when using the 'openpyxl', not the embedded formulae
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/example.xlsx
+++ b/py-polars/tests/unit/io/files/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/PycharmProjects/polars/py-polars/tests/unit/io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvis/GitHub/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CC5D58-BE66-1B40-ADAD-B654E84493A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89929A88-0E13-A846-A4D4-2FD349F8179E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10040" yWindow="12240" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6920" yWindow="9160" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>hello</t>
   </si>
@@ -62,13 +61,19 @@
     <t>Total</t>
   </si>
   <si>
-    <t>iter groups</t>
-  </si>
-  <si>
     <t>rows_by_key</t>
   </si>
   <si>
     <t>cardinality</t>
+  </si>
+  <si>
+    <t>iter_groups</t>
+  </si>
+  <si>
+    <t>!!!</t>
+  </si>
+  <si>
+    <t>:))</t>
   </si>
 </sst>
 </file>
@@ -78,11 +83,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -118,15 +130,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -295,9 +308,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0FCAA37-C0F1-2E4A-9449-70A700D0CF87}" name="Table1" displayName="Table1" ref="B5:D12" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B5:D11" xr:uid="{4B333195-25A9-3A4B-905B-074BF2160312}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter groups" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="2" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="4" totalsRowDxfId="1" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0" totalsRowCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -670,10 +683,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE632952-247C-8548-B0FE-C295508C7F03}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,13 +721,13 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -799,7 +812,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
-        <f>SUBTOTAL(109,Table1[iter groups])</f>
+        <f>SUBTOTAL(109,Table1[iter_groups])</f>
         <v>0.31331999999999999</v>
       </c>
       <c r="E12" s="2"/>
@@ -817,6 +830,21 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -831,7 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0923D58-9CA3-DE4B-90A8-4F460D7742EA}">
   <dimension ref="B5:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -842,18 +870,21 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="str">
+        <f>TEXT("cardinality","0")</f>
+        <v>cardinality</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>TEXT("rows_by_key","0")</f>
+        <v>rows_by_key</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>TEXT("iter_groups",0)</f>
+        <v>iter_groups</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -864,7 +895,7 @@
         <v>4.8059999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -875,7 +906,7 @@
         <v>4.2229999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>15</v>
       </c>
@@ -886,7 +917,7 @@
         <v>4.7739999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>30</v>
       </c>
@@ -897,7 +928,7 @@
         <v>4.8640000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>150</v>
       </c>
@@ -908,7 +939,7 @@
         <v>5.7200000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>300</v>
       </c>
@@ -919,7 +950,12 @@
         <v>6.9449999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
feat(python): support `pyxlsb` engine for reading binary workbooks with `read_excel`
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/example.xlsx
+++ b/py-polars/tests/unit/io/files/example.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvis/GitHub/polars/py-polars/tests/unit/io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/PycharmProjects/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89929A88-0E13-A846-A4D4-2FD349F8179E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856AF825-6EBE-EF42-AD0D-055AF191BC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="9160" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37900" yWindow="20060" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
     <sheet name="test2" sheetId="2" r:id="rId2"/>
     <sheet name="test3" sheetId="3" r:id="rId3"/>
     <sheet name="test4" sheetId="4" r:id="rId4"/>
+    <sheet name="test5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>hello</t>
   </si>
@@ -74,20 +75,38 @@
   </si>
   <si>
     <t>:))</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>dtm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -110,13 +129,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,22 +173,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B646C9DC-CF89-1844-B1F6-969631BBBD7F}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{D65B7284-0216-A64A-AC6B-2B9C645B72D5}"/>
     <cellStyle name="Per cent 2" xfId="2" xr:uid="{2DCABF6C-A3B8-464F-B265-6E3D296E4444}"/>
   </cellStyles>
   <dxfs count="8">
@@ -308,9 +363,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0FCAA37-C0F1-2E4A-9449-70A700D0CF87}" name="Table1" displayName="Table1" ref="B5:D12" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B5:D11" xr:uid="{4B333195-25A9-3A4B-905B-074BF2160312}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="2" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="4" totalsRowDxfId="1" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="3" totalsRowDxfId="2" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" totalsRowCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -615,14 +670,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -650,14 +703,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -685,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE632952-247C-8548-B0FE-C295508C7F03}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1170,4 +1221,58 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K737373 Classification: Public</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CCBD78-1211-5646-88B1-B0B72F3EDB7B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="7"/>
+    <col min="3" max="3" width="4.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>36525.438020833331</v>
+      </c>
+      <c r="B2" s="11">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>40462.509189814817</v>
+      </c>
+      <c r="B3" s="11">
+        <v>43319</v>
+      </c>
+      <c r="C3" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(python): Add "drop_empty_cols" parameter for `read_excel` and `read_ods`
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/example.xlsx
+++ b/py-polars/tests/unit/io/files/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/PycharmProjects/polars/py-polars/tests/unit/io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/Projects/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856AF825-6EBE-EF42-AD0D-055AF191BC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA245EC2-143C-7C44-B146-AF5533809050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37900" yWindow="20060" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="test4" sheetId="4" r:id="rId4"/>
     <sheet name="test5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>hello</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>iter_groups</t>
-  </si>
-  <si>
-    <t>!!!</t>
   </si>
   <si>
     <t>:))</t>
@@ -93,7 +90,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -193,7 +190,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,9 +369,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -412,7 +409,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -518,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -660,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -894,7 +891,7 @@
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -910,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0923D58-9CA3-DE4B-90A8-4F460D7742EA}">
   <dimension ref="B5:F49"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1002,9 +999,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C16" s="2"/>
@@ -1227,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CCBD78-1211-5646-88B1-B0B72F3EDB7B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
@@ -1241,13 +1236,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat(python): Add "drop_empty_cols" parameter for `read_excel` and `read_ods` (#20430)
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/example.xlsx
+++ b/py-polars/tests/unit/io/files/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/PycharmProjects/polars/py-polars/tests/unit/io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/Projects/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856AF825-6EBE-EF42-AD0D-055AF191BC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA245EC2-143C-7C44-B146-AF5533809050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37900" yWindow="20060" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="test4" sheetId="4" r:id="rId4"/>
     <sheet name="test5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>hello</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>iter_groups</t>
-  </si>
-  <si>
-    <t>!!!</t>
   </si>
   <si>
     <t>:))</t>
@@ -93,7 +90,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -193,7 +190,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,9 +369,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -412,7 +409,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -518,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -660,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -894,7 +891,7 @@
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -910,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0923D58-9CA3-DE4B-90A8-4F460D7742EA}">
   <dimension ref="B5:F49"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1002,9 +999,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C16" s="2"/>
@@ -1227,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CCBD78-1211-5646-88B1-B0B72F3EDB7B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
@@ -1241,13 +1236,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat(python): Improve internal string → temporal parsing in `read_excel`
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/example.xlsx
+++ b/py-polars/tests/unit/io/files/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/Projects/polars/py-polars/tests/unit/io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvis/GitHub/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA245EC2-143C-7C44-B146-AF5533809050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C2473-12A9-AA4E-9DB8-B4C65C7A62AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="2320" windowWidth="28920" windowHeight="20920" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,12 @@
     <sheet name="test3" sheetId="3" r:id="rId3"/>
     <sheet name="test4" sheetId="4" r:id="rId4"/>
     <sheet name="test5" sheetId="5" r:id="rId5"/>
+    <sheet name="temporal" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <definedNames>
+    <definedName name="TemporalTable">TemporalData[#All]</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>hello</t>
   </si>
@@ -81,18 +85,49 @@
   </si>
   <si>
     <t>dtm</t>
+  </si>
+  <si>
+    <t>2007-06-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2026-05-07 23:59:59</t>
+  </si>
+  <si>
+    <t>1900-01-30 14:50:20</t>
+  </si>
+  <si>
+    <t>tm_str</t>
+  </si>
+  <si>
+    <t>dt_str</t>
+  </si>
+  <si>
+    <t>dtm_str</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>2000-06-14</t>
+  </si>
+  <si>
+    <t>1978-02-28</t>
+  </si>
+  <si>
+    <t>2040-12-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -140,6 +175,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -176,7 +232,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -191,6 +247,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,7 +281,262 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{D65B7284-0216-A64A-AC6B-2B9C645B72D5}"/>
     <cellStyle name="Per cent 2" xfId="2" xr:uid="{2DCABF6C-A3B8-464F-B265-6E3D296E4444}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -357,21 +695,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0FCAA37-C0F1-2E4A-9449-70A700D0CF87}" name="Table1" displayName="Table1" ref="B5:D12" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0FCAA37-C0F1-2E4A-9449-70A700D0CF87}" name="Table1" displayName="Table1" ref="B5:D12" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="B5:D11" xr:uid="{4B333195-25A9-3A4B-905B-074BF2160312}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="3" totalsRowDxfId="2" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="19" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="18" totalsRowDxfId="17" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15" totalsRowCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A642ACF5-3B21-7446-8839-01FE81FA6BC6}" name="TemporalData" displayName="TemporalData" ref="B4:G8" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
+  <autoFilter ref="B4:G8" xr:uid="{A3154F86-352B-A644-9226-035082BB2103}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BA51FABA-A9FF-0A46-9A65-E29EDB173B22}" name="id" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C4D1E4C7-95C6-B344-B017-3492996B56F2}" name="dtm" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{A3E5C95B-8A29-B042-AF28-14D47A4E8D7B}" name="dt" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{EACA6BAE-DA2B-D44F-A5F1-77A023B46D94}" name="dtm_str" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{187C1D0B-0BF4-3E43-84F0-3FA22708D923}" name="dt_str" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A90B213B-052A-7140-BEFC-B3FE445A4427}" name="tm_str" dataDxfId="1" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark7" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -409,7 +762,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -515,7 +868,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -657,7 +1010,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -907,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0923D58-9CA3-DE4B-90A8-4F460D7742EA}">
   <dimension ref="B5:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1270,4 +1623,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D708565B-E16F-A447-8374-749F3835FF38}">
+  <dimension ref="B4:G8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="15">
+        <v>100</v>
+      </c>
+      <c r="C5" s="14">
+        <v>36525.043090277781</v>
+      </c>
+      <c r="D5" s="17">
+        <v>36543</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0.99331018518518521</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="15">
+        <v>200</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="17">
+        <v>23962</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="15">
+        <v>300</v>
+      </c>
+      <c r="C7" s="14">
+        <v>25389.438020833335</v>
+      </c>
+      <c r="D7" s="17">
+        <v>46499</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="19">
+        <v>0.42399305555555555</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="15">
+        <v>400</v>
+      </c>
+      <c r="C8" s="14">
+        <v>64933.249814814815</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.7710069444444444</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(python): Improve string → temporal parsing in `read_excel` and `read_ods` (#20845)
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/example.xlsx
+++ b/py-polars/tests/unit/io/files/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/Projects/polars/py-polars/tests/unit/io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvis/GitHub/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA245EC2-143C-7C44-B146-AF5533809050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C2473-12A9-AA4E-9DB8-B4C65C7A62AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="2320" windowWidth="28920" windowHeight="20920" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,12 @@
     <sheet name="test3" sheetId="3" r:id="rId3"/>
     <sheet name="test4" sheetId="4" r:id="rId4"/>
     <sheet name="test5" sheetId="5" r:id="rId5"/>
+    <sheet name="temporal" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <definedNames>
+    <definedName name="TemporalTable">TemporalData[#All]</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>hello</t>
   </si>
@@ -81,18 +85,49 @@
   </si>
   <si>
     <t>dtm</t>
+  </si>
+  <si>
+    <t>2007-06-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2026-05-07 23:59:59</t>
+  </si>
+  <si>
+    <t>1900-01-30 14:50:20</t>
+  </si>
+  <si>
+    <t>tm_str</t>
+  </si>
+  <si>
+    <t>dt_str</t>
+  </si>
+  <si>
+    <t>dtm_str</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>2000-06-14</t>
+  </si>
+  <si>
+    <t>1978-02-28</t>
+  </si>
+  <si>
+    <t>2040-12-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -140,6 +175,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -176,7 +232,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -191,6 +247,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,7 +281,262 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{D65B7284-0216-A64A-AC6B-2B9C645B72D5}"/>
     <cellStyle name="Per cent 2" xfId="2" xr:uid="{2DCABF6C-A3B8-464F-B265-6E3D296E4444}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -357,21 +695,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0FCAA37-C0F1-2E4A-9449-70A700D0CF87}" name="Table1" displayName="Table1" ref="B5:D12" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0FCAA37-C0F1-2E4A-9449-70A700D0CF87}" name="Table1" displayName="Table1" ref="B5:D12" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="B5:D11" xr:uid="{4B333195-25A9-3A4B-905B-074BF2160312}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="3" totalsRowDxfId="2" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="19" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="18" totalsRowDxfId="17" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15" totalsRowCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A642ACF5-3B21-7446-8839-01FE81FA6BC6}" name="TemporalData" displayName="TemporalData" ref="B4:G8" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
+  <autoFilter ref="B4:G8" xr:uid="{A3154F86-352B-A644-9226-035082BB2103}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BA51FABA-A9FF-0A46-9A65-E29EDB173B22}" name="id" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C4D1E4C7-95C6-B344-B017-3492996B56F2}" name="dtm" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{A3E5C95B-8A29-B042-AF28-14D47A4E8D7B}" name="dt" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{EACA6BAE-DA2B-D44F-A5F1-77A023B46D94}" name="dtm_str" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{187C1D0B-0BF4-3E43-84F0-3FA22708D923}" name="dt_str" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A90B213B-052A-7140-BEFC-B3FE445A4427}" name="tm_str" dataDxfId="1" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark7" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -409,7 +762,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -515,7 +868,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -657,7 +1010,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -907,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0923D58-9CA3-DE4B-90A8-4F460D7742EA}">
   <dimension ref="B5:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1270,4 +1623,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D708565B-E16F-A447-8374-749F3835FF38}">
+  <dimension ref="B4:G8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="15">
+        <v>100</v>
+      </c>
+      <c r="C5" s="14">
+        <v>36525.043090277781</v>
+      </c>
+      <c r="D5" s="17">
+        <v>36543</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0.99331018518518521</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="15">
+        <v>200</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="17">
+        <v>23962</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1.1574074074074073E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="15">
+        <v>300</v>
+      </c>
+      <c r="C7" s="14">
+        <v>25389.438020833335</v>
+      </c>
+      <c r="D7" s="17">
+        <v>46499</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="19">
+        <v>0.42399305555555555</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="15">
+        <v>400</v>
+      </c>
+      <c r="C8" s="14">
+        <v>64933.249814814815</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.7710069444444444</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>